<commit_message>
new calculations with new timeseries
</commit_message>
<xml_diff>
--- a/Three node models/in.xlsx
+++ b/Three node models/in.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e0338d3ac8c54621/GitHub/Locational-investment-signals/Three node models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.eicke\Documents\Locational-investment-signals\Three node models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{DB235AB6-003E-4497-8B2B-DD716646F744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67A522A5-B1EE-4F62-8AD8-A754F0D00797}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB636F1-D98F-4E2F-91D1-379A34C5F0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cost" sheetId="2" r:id="rId1"/>
@@ -770,7 +770,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -919,10 +919,10 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>231.4</c:v>
+                  <c:v>603.07999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -985,7 +985,7 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>583.12</c:v>
+                  <c:v>679.48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1051,7 +1051,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="589632111"/>
@@ -1111,7 +1111,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="589627951"/>
@@ -1152,7 +1152,7 @@
       <a:pPr>
         <a:defRPr sz="1100"/>
       </a:pPr>
-      <a:endParaRPr lang="en-DE"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1204,7 +1204,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1250,16 +1250,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="48"/>
                 <c:pt idx="0">
-                  <c:v>0.37</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35</c:v>
+                  <c:v>0.51</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.32</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.31</c:v>
+                  <c:v>0.33</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.28000000000000003</c:v>
@@ -1274,22 +1274,22 @@
                   <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.27</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.19</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.15</c:v>
+                  <c:v>0.11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.09</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.11</c:v>
@@ -1298,25 +1298,25 @@
                   <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.13</c:v>
+                  <c:v>0.18</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.17</c:v>
+                  <c:v>0.28999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.21</c:v>
+                  <c:v>0.36</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.25</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.28999999999999998</c:v>
+                  <c:v>0.38</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.22</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.19</c:v>
+                  <c:v>0.26</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0.21</c:v>
@@ -1481,25 +1481,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.01</c:v>
+                  <c:v>0.11</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.17</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0.28000000000000003</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.22</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.03</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>0</c:v>
@@ -1628,28 +1628,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="48"/>
                 <c:pt idx="0">
-                  <c:v>0.16</c:v>
+                  <c:v>0.51</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.18</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.17</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.14000000000000001</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.09</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.12</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.17</c:v>
@@ -1658,46 +1658,46 @@
                   <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.15</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>0.16</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>0.17</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.18</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.17</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.15</c:v>
-                </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.15</c:v>
+                  <c:v>0.31</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.17</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.18</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>0.18</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.22</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.25</c:v>
+                  <c:v>0.11</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0.28000000000000003</c:v>
@@ -1868,10 +1868,10 @@
                   <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.49</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.47</c:v>
+                  <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0.38</c:v>
@@ -2023,7 +2023,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="509294543"/>
@@ -2082,7 +2082,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="509296207"/>
@@ -2124,7 +2124,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2154,7 +2154,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-DE"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2205,7 +2205,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2685,7 +2685,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="509307439"/>
@@ -2744,7 +2744,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="509309103"/>
@@ -2786,7 +2786,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2816,7 +2816,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-DE"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4918,8 +4918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5047,21 +5047,21 @@
         <v>0.32</v>
       </c>
       <c r="G5" s="42">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H5" s="40">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="N5" s="28" t="s">
         <v>13</v>
       </c>
       <c r="O5" s="12">
         <f>G5</f>
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P5" s="13">
         <f t="shared" ref="P5" si="0">G5+H5*$P$4/1000</f>
-        <v>231.4</v>
+        <v>603.07999999999993</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="16.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5084,7 +5084,7 @@
         <v>40</v>
       </c>
       <c r="H6" s="40">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="N6" s="28" t="s">
         <v>14</v>
@@ -5095,7 +5095,7 @@
       </c>
       <c r="P6" s="15">
         <f>G6+H6*$P$4/1000</f>
-        <v>583.12</v>
+        <v>679.48</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="16.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5115,7 +5115,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="42">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="H7" s="40">
         <f>E7/D7+F7/D7*$C$33</f>
@@ -5141,7 +5141,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="10"/>
       <c r="G8" s="42">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H8" s="40">
         <v>0</v>
@@ -5307,8 +5307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58BF2839-4BDE-4B18-A7A4-A5F1FDEE19B7}">
   <dimension ref="B1:Y95"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O46" sqref="O46"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5387,13 +5387,13 @@
         <v>1</v>
       </c>
       <c r="F4" s="45">
-        <v>0.37</v>
+        <v>0.67</v>
       </c>
       <c r="G4" s="45">
         <v>0</v>
       </c>
       <c r="H4" s="45">
-        <v>0.16</v>
+        <v>0.51</v>
       </c>
       <c r="I4" s="45">
         <v>0</v>
@@ -5413,13 +5413,13 @@
         <v>2</v>
       </c>
       <c r="F5" s="45">
-        <v>0.35</v>
+        <v>0.51</v>
       </c>
       <c r="G5" s="45">
         <v>0</v>
       </c>
       <c r="H5" s="45">
-        <v>0.18</v>
+        <v>0.42</v>
       </c>
       <c r="I5" s="45">
         <v>0</v>
@@ -5443,13 +5443,13 @@
         <v>3</v>
       </c>
       <c r="F6" s="45">
-        <v>0.32</v>
+        <v>0.4</v>
       </c>
       <c r="G6" s="45">
         <v>0.03</v>
       </c>
       <c r="H6" s="45">
-        <v>0.17</v>
+        <v>0.33</v>
       </c>
       <c r="I6" s="45">
         <v>0</v>
@@ -5473,13 +5473,13 @@
         <v>4</v>
       </c>
       <c r="F7" s="45">
-        <v>0.31</v>
+        <v>0.33</v>
       </c>
       <c r="G7" s="45">
         <v>0.12</v>
       </c>
       <c r="H7" s="45">
-        <v>0.14000000000000001</v>
+        <v>0.18</v>
       </c>
       <c r="I7" s="45">
         <v>0.02</v>
@@ -5509,7 +5509,7 @@
         <v>0.25</v>
       </c>
       <c r="H8" s="45">
-        <v>0.09</v>
+        <v>0.15</v>
       </c>
       <c r="I8" s="45">
         <v>0.13</v>
@@ -5539,7 +5539,7 @@
         <v>0.31</v>
       </c>
       <c r="H9" s="45">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="I9" s="45">
         <v>0.23</v>
@@ -5569,7 +5569,7 @@
         <v>0.32</v>
       </c>
       <c r="H10" s="45">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="I10" s="45">
         <v>0.21</v>
@@ -5599,7 +5599,7 @@
         <v>0.26</v>
       </c>
       <c r="H11" s="45">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="I11" s="45">
         <v>0.12</v>
@@ -5623,7 +5623,7 @@
         <v>9</v>
       </c>
       <c r="F12" s="45">
-        <v>0.27</v>
+        <v>0.2</v>
       </c>
       <c r="G12" s="45">
         <v>0.09</v>
@@ -5653,7 +5653,7 @@
         <v>10</v>
       </c>
       <c r="F13" s="45">
-        <v>0.19</v>
+        <v>0.15</v>
       </c>
       <c r="G13" s="45">
         <v>0</v>
@@ -5683,13 +5683,13 @@
         <v>11</v>
       </c>
       <c r="F14" s="45">
-        <v>0.15</v>
+        <v>0.11</v>
       </c>
       <c r="G14" s="45">
         <v>0</v>
       </c>
       <c r="H14" s="45">
-        <v>0.14000000000000001</v>
+        <v>0.13</v>
       </c>
       <c r="I14" s="45">
         <v>0</v>
@@ -5713,13 +5713,13 @@
         <v>12</v>
       </c>
       <c r="F15" s="45">
-        <v>0.12</v>
+        <v>0.04</v>
       </c>
       <c r="G15" s="45">
         <v>0</v>
       </c>
       <c r="H15" s="45">
-        <v>0.15</v>
+        <v>0.06</v>
       </c>
       <c r="I15" s="45">
         <v>0</v>
@@ -5743,13 +5743,13 @@
         <v>13</v>
       </c>
       <c r="F16" s="45">
-        <v>0.09</v>
+        <v>0.02</v>
       </c>
       <c r="G16" s="45">
         <v>0</v>
       </c>
       <c r="H16" s="45">
-        <v>0.16</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="I16" s="45">
         <v>0</v>
@@ -5773,13 +5773,13 @@
         <v>14</v>
       </c>
       <c r="F17" s="45">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="G17" s="45">
         <v>0</v>
       </c>
       <c r="H17" s="45">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
       <c r="I17" s="45">
         <v>0</v>
@@ -5806,10 +5806,10 @@
         <v>0.11</v>
       </c>
       <c r="G18" s="45">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="H18" s="45">
-        <v>0.18</v>
+        <v>0.13</v>
       </c>
       <c r="I18" s="45">
         <v>0.04</v>
@@ -5836,10 +5836,10 @@
         <v>0.15</v>
       </c>
       <c r="G19" s="45">
-        <v>0.01</v>
+        <v>0.11</v>
       </c>
       <c r="H19" s="45">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="I19" s="45">
         <v>0.18</v>
@@ -5863,13 +5863,13 @@
         <v>17</v>
       </c>
       <c r="F20" s="45">
-        <v>0.13</v>
+        <v>0.18</v>
       </c>
       <c r="G20" s="45">
+        <v>0.24</v>
+      </c>
+      <c r="H20" s="45">
         <v>0.17</v>
-      </c>
-      <c r="H20" s="45">
-        <v>0.15</v>
       </c>
       <c r="I20" s="45">
         <v>0.39</v>
@@ -5893,16 +5893,16 @@
         <v>18</v>
       </c>
       <c r="F21" s="45">
-        <v>0.17</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="G21" s="45">
-        <v>0.28000000000000003</v>
+        <v>0.32</v>
       </c>
       <c r="H21" s="45">
-        <v>0.14000000000000001</v>
+        <v>0.21</v>
       </c>
       <c r="I21" s="45">
-        <v>0.49</v>
+        <v>0.45</v>
       </c>
       <c r="V21" s="59"/>
       <c r="W21" s="60"/>
@@ -5923,16 +5923,16 @@
         <v>19</v>
       </c>
       <c r="F22" s="45">
-        <v>0.21</v>
+        <v>0.36</v>
       </c>
       <c r="G22" s="45">
-        <v>0.22</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H22" s="45">
-        <v>0.15</v>
+        <v>0.31</v>
       </c>
       <c r="I22" s="45">
-        <v>0.47</v>
+        <v>0.42</v>
       </c>
       <c r="V22" s="59"/>
       <c r="W22" s="60"/>
@@ -5953,13 +5953,13 @@
         <v>20</v>
       </c>
       <c r="F23" s="45">
-        <v>0.25</v>
+        <v>0.45</v>
       </c>
       <c r="G23" s="45">
-        <v>0.03</v>
+        <v>0.13</v>
       </c>
       <c r="H23" s="45">
-        <v>0.17</v>
+        <v>0.45</v>
       </c>
       <c r="I23" s="45">
         <v>0.38</v>
@@ -5983,13 +5983,13 @@
         <v>21</v>
       </c>
       <c r="F24" s="45">
-        <v>0.28999999999999998</v>
+        <v>0.38</v>
       </c>
       <c r="G24" s="45">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="H24" s="45">
-        <v>0.18</v>
+        <v>0.32</v>
       </c>
       <c r="I24" s="45">
         <v>0.15</v>
@@ -6013,7 +6013,7 @@
         <v>22</v>
       </c>
       <c r="F25" s="45">
-        <v>0.22</v>
+        <v>0.3</v>
       </c>
       <c r="G25" s="45">
         <v>0</v>
@@ -6043,13 +6043,13 @@
         <v>23</v>
       </c>
       <c r="F26" s="45">
-        <v>0.19</v>
+        <v>0.26</v>
       </c>
       <c r="G26" s="45">
         <v>0</v>
       </c>
       <c r="H26" s="45">
-        <v>0.22</v>
+        <v>0.13</v>
       </c>
       <c r="I26" s="45">
         <v>0</v>
@@ -6079,7 +6079,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="45">
-        <v>0.25</v>
+        <v>0.11</v>
       </c>
       <c r="I27" s="45">
         <v>0</v>
@@ -6311,11 +6311,11 @@
       </c>
       <c r="M35" s="47">
         <f>N43</f>
-        <v>1905.3</v>
+        <v>2270.3000000000002</v>
       </c>
       <c r="N35" s="47">
         <f>P43</f>
-        <v>1397.9500000000003</v>
+        <v>1755.6499999999999</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.35">
@@ -6348,11 +6348,11 @@
       </c>
       <c r="M36" s="47">
         <f>O43</f>
-        <v>762.85</v>
+        <v>923.45</v>
       </c>
       <c r="N36" s="47">
         <f>Q43</f>
-        <v>1043.8999999999999</v>
+        <v>1011.0499999999998</v>
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.35">
@@ -6565,19 +6565,19 @@
       </c>
       <c r="N43" s="51">
         <f>(8760*N44)</f>
-        <v>1905.3</v>
+        <v>2270.3000000000002</v>
       </c>
       <c r="O43" s="51">
         <f t="shared" ref="O43:Q43" si="0">(8760*O44)</f>
-        <v>762.85</v>
+        <v>923.45</v>
       </c>
       <c r="P43" s="51">
         <f t="shared" si="0"/>
-        <v>1397.9500000000003</v>
+        <v>1755.6499999999999</v>
       </c>
       <c r="Q43" s="51">
         <f t="shared" si="0"/>
-        <v>1043.8999999999999</v>
+        <v>1011.0499999999998</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.35">
@@ -6610,19 +6610,19 @@
       </c>
       <c r="N44" s="52">
         <f>AVERAGE(F4:F27)</f>
-        <v>0.2175</v>
+        <v>0.25916666666666671</v>
       </c>
       <c r="O44" s="52">
         <f>AVERAGE(G4:G27)</f>
-        <v>8.7083333333333332E-2</v>
+        <v>0.10541666666666667</v>
       </c>
       <c r="P44" s="52">
         <f>AVERAGE(H4:H27)</f>
-        <v>0.15958333333333335</v>
+        <v>0.20041666666666666</v>
       </c>
       <c r="Q44" s="52">
         <f>AVERAGE(I4:I27)</f>
-        <v>0.11916666666666664</v>
+        <v>0.11541666666666665</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.35">
@@ -6677,10 +6677,10 @@
         <v>0.53</v>
       </c>
       <c r="N46" s="45">
-        <v>2500</v>
+        <v>2200</v>
       </c>
       <c r="P46" s="45">
-        <v>2000</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.35">

</xml_diff>